<commit_message>
* First revamp of mapping BHealSc Outcomes to Learning Objectives for papers.
</commit_message>
<xml_diff>
--- a/2022 Major - Papers - Outcome Map.xlsx
+++ b/2022 Major - Papers - Outcome Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/BHealSc/Shared Documents/Administration/Curriculum Mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/BHealSc/Shared Documents/Scripts/Major Paper Outcomes Script/BHealSc Curriculum Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="557" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AA0398C-2CB3-4B70-AD23-1BE45CFD54B7}"/>
+  <xr:revisionPtr revIDLastSave="730" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1178F0B5-DA58-4FF6-B86C-A829F7DDF848}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="314">
   <si>
     <t>Paper</t>
   </si>
@@ -1726,13 +1726,321 @@
   </si>
   <si>
     <t>Assessment 1 (Presentation - Culture in Action); Policy Report (2500 words); Group Assignment (Report and Presentation); Final Exam (2-hr)</t>
+  </si>
+  <si>
+    <t>CMHC_Detail</t>
+  </si>
+  <si>
+    <t>MAOH_Detail</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Have a capacity to build and manage relationships with colleagues, organisations, individuals and families/whānau, through a capacity to listen, validate concerns, ask appropriate questions, maintain personal boundaries, and respond helpfully with empathy and respectful directness.&lt;/li&gt;&lt;li&gt;When working with individuals and families/whānau, be able to identify needs and help them access services.&lt;/li&gt;&lt;li&gt;Communicate with competence across all media.&lt;/li&gt;&lt;b&gt;&lt;li&gt;When working with Māori individuals, whānau, organisations and communities, be able to utilise models of engagement and communication that foster positive outcomes within healthcare and public health settings.&lt;/li&gt;&lt;li&gt;Have an understanding of the importance of Te Reo Māori within the context of health care.&lt;/li&gt;&lt;li&gt;Demonstrate the capacity to form a positive relationship with Māori individuals and whānau within a health setting including utilising appropriate pronunciation of Te Reo Māori.&lt;/li&gt;&lt;li&gt;Demonstrate the capacity to write and say an appropriate mihimihi that could be used in a health setting.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Understand and apply strong ethical principles in their work,
+including requirements for privacy and confidentiality.&lt;/li&gt;&lt;li&gt;Understand, value, consider and respect the roles of various health providers and organisations.&lt;/li&gt;&lt;li&gt;Have knowledge of the theories and models of health and disability, including peoples’ rights.&lt;/li&gt;&lt;b&gt;&lt;li&gt;Knowledge of ethics as it applies to Māori health services and research.&lt;/li&gt;&lt;li&gt;Capacity to identify how to respond to ethics expectations of health research involving Māori.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Appreciate the Treaty of Waitangi and its importance and relationship with both individual and public health.&lt;/li&gt;&lt;li&gt;Understand cultural diversity and multi culturalism both globally and in New Zealand.&lt;/li&gt;&lt;b&gt;&lt;li&gt;To have knowledge of Te Tiriti or Waitangi articles and principles and their application in supporting Māori health outcomes.&lt;/li&gt;&lt;li&gt;Understand concepts of cultural competence, cultural safety and structural competency and be able to apply these concepts when addressing Māori health.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Gather relevant and required health information from populations and/or an individual, their family/whānau, their health providers, and involved organisations relevant to their health needs.&lt;/li&gt;&lt;li&gt;Assimilate, filter and critically analyse a broad range of health, financial, cultural, and social information related to individuals, groups and populations.&lt;/li&gt;&lt;b&gt;&lt;li&gt;To have a sound understanding of key sources of information on Māori health and be able to demonstrate an understanding of critical analysis of health research informing on Māori health.&lt;/li&gt;&lt;li&gt;To have an understanding of concepts of implicit and explicit bias, unconscious bias and identify the impact of this bias on interpretations of Māori health outcomes.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Have a broad understanding of the complex and multiple influences on health and disability including determinants and outcomes.&lt;/li&gt;&lt;li&gt;Work across the spectrum of illness, injury, health and disability needs, with individuals, families/whanau, communities and populations, which may include: physical, psychological, social, cultural, intellectual and environmental components.&lt;/li&gt;&lt;li&gt;Have knowledge of health in a global context.&lt;/li&gt;&lt;b&gt;&lt;li&gt;To be able to apply important public health frameworks to important health issues impacting on Māori.&lt;/li&gt;&lt;li&gt;To have an understanding of Māori population health and inequity, and identify key public health strategies to reduce health inequity.&lt;/li&gt;&lt;li&gt;To have a sound understanding of the concepts of health inequality and inequity and be able to describe the determinants and solutions to addressing Māori health inequity.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;li&gt;To have knowledge of Māori health issues impacting at different stages of the lifecourse including pregnancy, childbirth, infancy, childhood, adolescence, adulthood and older ages.&lt;/li&gt;&lt;li&gt;To understand tikanga associated with key aspects of the life course including childbirth, death and dying.&lt;/li&gt;&lt;li&gt;To have an understanding of key areas of the health and social service sector that are responsive to Māori needs at key phases of the lifecourse, from pregnancy through to kaumatua services.&lt;/li&gt;&lt;li&gt;To be able to describe the concept of Hauora, including models of Hauora and how these can be used to explore Māori health and wellbeing.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Have a working knowledge of key health conditions and health needs.&lt;/li&gt;&lt;li&gt;Understand the distribution of key health conditions in various communities and situations.&lt;/li&gt;&lt;li&gt;When working with individuals and families/whānau:&lt;ol type='1'&gt;&lt;li&gt;Understand sufficiently a person’s health and disability, and the impact on their lives.&lt;/li&gt;&lt;li&gt;Have sufficient knowledge to be able to negotiate appropriate care and rehabilitation with providers on behalf of the person.&lt;/li&gt;&lt;/ol&gt;&lt;/li&gt;&lt;li&gt;Understand in general terms what the required investigations, treatments, and management for individual patients or groups of patients may be.&lt;/li&gt;&lt;b&gt;&lt;li&gt;Have a working knowledge of key health conditions and health needs, in particular those conditions impacting on Māori, including the determinants and solutions to addressing areas of health inequity.&lt;/li&gt;&lt;li&gt;Understand the distribution of key health conditions in Māori.&lt;/li&gt;&lt;li&gt;Identify current policies and strategies utilised in the health and social sectors aimed at addressing key health issues in Māori.&lt;/li&gt;&lt;li&gt;To have an understanding of the concepts surrounding disability from a Māori perspective and be able to describe approaches taken in disability support that reflect responsiveness to Māori.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Work competently in teams and networks, with the capacity to build relationships.&lt;/li&gt;&lt;li&gt;When working with individuals and families/whānau:&lt;ol type='1'&gt;&lt;li&gt;Draw together and coordinate care between providers, reducing duplication and sharing knowledge and information when needed, keeping the person at the centre of the process, and assisting them to live independently.&lt;/li&gt;&lt;/ol&gt;&lt;/li&gt;&lt;li&gt;When working with communities or groups:&lt;ol type='1'&gt;&lt;li&gt;Have a capacity to coordinate information between organisations and assist in generating collective responses to health issues.&lt;/li&gt;&lt;/ol&gt;&lt;/li&gt;&lt;b&gt;&lt;li&gt;Work effectively as a team member and with diverse communities and groups.&lt;/li&gt;&lt;li&gt;Demonstrate the capacity to work together in ways that are consistent with Māori values including whakawhanaungatanga and manaakitanga.&lt;/li&gt;&lt;li&gt;Discuss approaches taken within healthcare settings to foster positive partnerships with Māori including Māori whānau, marae, communities and organisations.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;When working with individuals and families/whānau:&lt;ol type='1'&gt;&lt;li&gt;Record and document information, assessment, and care planning fully and accurately.&lt;/li&gt;&lt;/ol&gt;&lt;/li&gt;&lt;li&gt;When working with communities or groups:&lt;ol type='1'&gt;&lt;li&gt;Locate, document and synthesise information about public health issues and appropriate interventions fully and accurately.&lt;/li&gt;&lt;/ol&gt;&lt;/li&gt;&lt;b&gt;&lt;li&gt;Understand the importance of accurate and consistent ethnicity data and describe approaches to ensuring quality of ethnicity data collection and analysis within a New Zealand context.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;When working with individuals and families/whānau:&lt;ol type="1"&gt;&lt;li&gt;Have an ability to manage complexity, particularly in the psychosocial area.&lt;/li&gt;&lt;li&gt;Manage the role of care manager working with individuals and families/whānau, as well as representative of a funding organisation.&lt;/li&gt;&lt;li&gt;Manage conflict.&lt;/li&gt;&lt;/ol&gt;&lt;/li&gt;&lt;li&gt;When working with communities or groups:&lt;ol type='1'&gt;&lt;li&gt;Have an ability to manage complexity, particularly in the psychosocial area.&lt;/li&gt;&lt;li&gt;Manage conflict.&lt;/li&gt;&lt;/ol&gt;&lt;/li&gt;&lt;b&gt;&lt;li&gt;Have an understanding of the broader interdisciplinary team involved in addressing Māori health including the regulated and non-regulated workforce.&lt;/li&gt;&lt;li&gt;Be able to describe the role of traditional Māori healers within contemporary health and social services today.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;li&gt;Understand the impact of changes in employment and income on trends in Māori health outcomes.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Be familiar with the New Zealand health system and its comparison to those overseas.&lt;/li&gt;&lt;li&gt;Have a working knowledge of legislation, regulations and research evidence relevant to health.&lt;/li&gt;&lt;li&gt;Understand the key agencies and entities involved in health quality.&lt;/li&gt;&lt;li&gt;Understand the political and global context of health and disability, and how this impacts on health policy, the delivery of health and social services, and service users.&lt;/li&gt;&lt;b&gt;&lt;li&gt;Have an understanding of the development and diversity of Māori health providers.&lt;/li&gt;&lt;li&gt;Be able to describe the challenges and opportunities faced by Māori health providers in meeting the diverse health needs of Māori.&lt;/li&gt;&lt;li&gt;Identify key determinants of health impacting on Māori and have an understanding of the relationships between health and social services in meeting the needs of Māori.&lt;/li&gt;&lt;li&gt;Be able to describe the Whānau Ora policy and its impacts on the development and delivery of health and social services to Māori.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Be committed to the fundamental importance of the acquisition and development of knowledge and understanding.&lt;/li&gt;&lt;li&gt;Be committed to the on-going acquisition of new knowledge and new skills, and an ability to apply these to an ever-changing environment.&lt;/li&gt;&lt;li&gt;Understand principles of quality care and have knowledge of and commitment to continuous quality improvement.&lt;/li&gt;&lt;b&gt;&lt;li&gt;Have an understanding of the relationship between matauranga Māori and Western knowledge systems.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Use knowledge of relevant research literature in the service of &lt;b&gt;Māori&lt;/b&gt; communities, the individual and employers, and be able to research, critically appraise and apply knowledge from new research in their work.&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;li&gt;Demonstrate the capacity to convey key health information to a Māori audience.&lt;/li&gt;&lt;li&gt;Be able to discuss the concept of health literacy and how it applies to supporting Māori health outcomes.&lt;/li&gt;&lt;li&gt;Have the capacity to develop and convey public health and individual health messages to Māori in ways that demonstrate understanding of te Ao Māori and Māori world views.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;&lt;li&gt;Demonstrate how you would integrate learning on Māori health when working with Māori individuals, whānau, communities, organisations and populations in order to achieve health gain for Māori.&lt;/li&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>PACH_Detail</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Understand and apply strong ethical principles in their work,
+including requirements for privacy and confidentiality.&lt;/li&gt;&lt;li&gt;Understand, value, consider and respect the roles of various health providers and organisations.&lt;/li&gt;&lt;li&gt;Have knowledge of the theories and models of health and disability, including &lt;b&gt;health equity&lt;/b&gt; and peoples’ rights.&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Terms_Tutorials</t>
+  </si>
+  <si>
+    <t>Demonstrate an attitude towards disabled people and people with long-term conditions that respects the individual and fosters a client-centred approach.;Understand the epidemiology of long-term conditions and disability in New Zealand.;Understand the concept of wellness and the role of healthy lifestyles to perpetuate wellness for people living with a long-term condition or disability.;Critically debate and discuss the different models of health care - for example, the International Classification of Functioning, Disability and Health-based biopsychosocial model, the social model, the recovery model for mental health, and Māori and Pacific models of health care.;Demonstrate a critical understanding of how non-health factors affect the experience of living with a long-term condition and disability.;Critically understand the interaction between mental, emotional and physical health and the effect that this may have on living with disability.;Understand the various approaches to determine functional status.;Understand and apply ethical decision making and discuss the principles of inter-professional professional practice.;A critical understanding of the process of goal-setting and the evaluation of outcome.</t>
+  </si>
+  <si>
+    <t>Discuss what is meant by health and health promotion.;Describe approaches to the planning, implementation and evaluation of health promotion activities.;Understand the role of the Ottawa Charter as providing a framework for different health promotion actions.;Understand how Te Tiriti o Waitangi, and ideas of social justice and ethics contribute to the practice of health promotion in Aotearoa New Zealand.;Identify the underlying principles of different health promotion activities and analyse their potential usefulness in achieving positive health outcomes.;Discuss, for specific health problems, the advantages and disadvantages of health promotion through education, community action and healthy public policy.</t>
+  </si>
+  <si>
+    <t>Demonstrate an understanding of the process and politics of health policymaking, including the main actors in the health policy process.;Demonstrate an understanding of frameworks for analysing health policy and health systems.;Demonstrate an understanding of different health systems and the various means by which health services are organised, funded and delivered in different countries.;Analyse and discuss various health policy issues and cases.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Assignment 1 (3000 words); Verbal Presentation; Final Exam (3-hr)</t>
+  </si>
+  <si>
+    <t>Assignment 1 (Project Plan Part 1); Assignment 2 (Project Plan Part 2); Final Exam (3-hr)</t>
+  </si>
+  <si>
+    <t>Assignment 1 (1500 words);A Assignment 2 (2000 words); Final Exam (3-hr)</t>
+  </si>
+  <si>
+    <t>Online Quiz; Group Presenation; Online Quiz; Assignment; Final Exam (1.5-hr)</t>
+  </si>
+  <si>
+    <t>10%;15%;10%;25%;40%</t>
+  </si>
+  <si>
+    <t>Demonstrate an understanding of key historical processes, personalities and events relating to Hauora Māori and Hauora a Iwi/Māori public health.;Critically examine the impact of historical factors on contemporary Hauora Māori and Hauora a Iwi/Māori public health outcomes.Demonstrate an understanding of contemporary Hauora Māori and Hauora a Iwi/Māori public health.;Critically analyse and understand contemporary Hauora Māori topics and public health approaches to addressing inequities.</t>
+  </si>
+  <si>
+    <t>Demonstrate an in-depth understanding of epidemiological concepts.;Describe the distribution, determinants, and prospects for control of specific important global health conditions.;Undertake a literature review of the epidemiology of a specific problem (exposure or disease/injury).;Describe a Public Health approach to the control of major health problems.;Understand the importance of a population approach to understanding health and disease in order to inform policies that promote health equity.;Understand the range of determinants of health, from genetic and individual behaviour to social and political influences.;Understand the importance of a range of strategies for the control of health problems including, but not limited to, the provision of health care.;Understand that epidemiology is the science that informs Public Health action – not an intellectual pursuit on its own.</t>
+  </si>
+  <si>
+    <t>Assignment Proposal; Assignment (3000 words); Final Exam (3-hr)</t>
+  </si>
+  <si>
+    <t>5%;35%;60%</t>
+  </si>
+  <si>
+    <t>Critically appraise relevant research on determinants and population health effects using public health models.;Develop, and effectively communicate, ideas about the key components of public and global health issues.;Identify effective public health strategies to address the issues.;Make recommendations for effective, integrated, multi-sectoral, collaborative approaches to public and global health issues.</t>
+  </si>
+  <si>
+    <t>Assignment 1 (2000 words); Assignment 2 (2000 words); Final Exam (3-hr)</t>
+  </si>
+  <si>
+    <t>25%;25%;50%</t>
+  </si>
+  <si>
+    <t>5%;5%;15%;35%;40%</t>
+  </si>
+  <si>
+    <t>Online Quiz 1A; Online Quiz 1B; Research Proposal (200 words); Research Report (1800 words); Final Exam (2-hr)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Presentation; Feedback Exercise; Quantitative Assignment; Qualitative Assignment</t>
+  </si>
+  <si>
+    <t>15%;5%;45%;35%</t>
+  </si>
+  <si>
+    <t>Demonstrate an understanding of the principles of research design and methodology specific to answering different types of research questions.;Distinguish between different methods of implementing research and justify the use of particular methods in different research situations.;Identify ethical and cultural issues related to research.;Demonstrate critical reflection on your own research and that of others.;Demonstrate an ability to communicate your research clearly.;Describe and present basic quantitative data using common spreadsheet software.;Demonstrate an understanding of qualitative research methods.</t>
+  </si>
+  <si>
+    <t>IA_Details_1</t>
+  </si>
+  <si>
+    <t>Ethics assignment:
+1. Define and explain the ethical concepts of beneficence, non-maleficence,
+autonomy and justice.
+2. Choose one of the three case studies presented in tutorial 2. Which of the ethical concepts are 
+relevant in this case? Explain why you think these concepts are pertinent in this particular case 
+study.
+3. Using the relevant concept/s, explain what you think should be done? Justify
+your answer.</t>
+  </si>
+  <si>
+    <t>IA_Details_2</t>
+  </si>
+  <si>
+    <t>Development assignment:
+You are a case worker in a medical centre where you are required to access support
+for children whose development is not progressing at a standard rate.
+1. Choose either early childhood or middle childhood as a focus age-group.
+2. Briefly outline what would be usually expected of a child of the chosen age group in the domains 
+of physical, cognitive, language and social development. You may bullet point this section of your 
+assignment.
+3. Imagine that you have been contacted by a family member of a child whose development in one of 
+these domains is not progressing satisfactorily: Describe the background, the whānau/family’s 
+concerns and what you observe in your interactions with the child and their caregiver. NB: you will 
+need to construct this hypothetical ‘case study’ from what you have learnt about usual 
+developmental processes.
+4. What support services are available in Aotearoa/New Zealand for this
+whānau/family?</t>
+  </si>
+  <si>
+    <t>IA_Details_3</t>
+  </si>
+  <si>
+    <t>Groups for this assignment will be formed in the week 1 tutorial session. The group
+will be required to demonstrate their understanding of the basic science and sociocultural
+factors of a case study developed by them. Students will be expected to
+present their knowledge of the condition, medical treatment options, psychosocial
+treatment options and complementary and alternative treatment options. This is to be
+presented to your tutorial group in tutorial 8 (in week 10 of the course). In the tutorial
+you will also complete a reflection on the input and commitment of the members of
+your group. This will be taken into consideration in the marking of your presentation.</t>
+  </si>
+  <si>
+    <t>IA_Details_4</t>
+  </si>
+  <si>
+    <t>IA_Details_5</t>
+  </si>
+  <si>
+    <t>Describe and understand the multidimensional nature of lifespan development;Demonstrate an understanding of context on human development;Have  an  awareness  of  the  healthcare  services  available  to  people  at  different stages of life;Analyse and discuss a range of health-related case studies;Understand ethical concepts and be able to apply them in healthcare settings;Be  aware  of  difference  (culture,  gender,  age,  sexuality,  disability)  and be conscious of your own biases;Have good listening and communication  skills and understand professional boundaries.</t>
+  </si>
+  <si>
+    <t>IA_Outcomes_1</t>
+  </si>
+  <si>
+    <t>IA_Outcomes_2</t>
+  </si>
+  <si>
+    <t>IA_Outcomes_3</t>
+  </si>
+  <si>
+    <t>IA_Outcomes_4</t>
+  </si>
+  <si>
+    <t>IA_Outcomes_5</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;b&lt;/b&gt; Ethical knowledge and practice &lt;br /&gt;&lt;b&gt;d&lt;/b&gt; Information gathering and critical analysis &lt;br /&gt;&lt;b&gt;f&lt;/b&gt; Knowledge of health human development and functioning &lt;br /&gt;&lt;b&gt;n&lt;/b&gt; Quality and safety in practice &lt;br /&gt;</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_1</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_2</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_3</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_4</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_5</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_6</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_7</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_8</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_9</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_10</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_11</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_12</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_13</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_14</t>
+  </si>
+  <si>
+    <t>LO_Outcomes_15</t>
+  </si>
+  <si>
+    <t>d;f</t>
+  </si>
+  <si>
+    <t>c;d;f</t>
+  </si>
+  <si>
+    <t>c;d;f;n</t>
+  </si>
+  <si>
+    <t>a;b;c;d;f;n;o</t>
+  </si>
+  <si>
+    <t>b;c;d</t>
+  </si>
+  <si>
+    <t>c;f</t>
+  </si>
+  <si>
+    <t>a;c;n</t>
+  </si>
+  <si>
+    <t>BHealSc_Outcomes</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;f;g;h;I;j;l;m;n;o;p</t>
+  </si>
+  <si>
+    <t>a;b;c;d;f;g;h;I;m;n;o;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;f;g;h;I;j;k;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;f;g;h;I;j;l;m;n;o;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;I;j;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;I;k;l;m</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;I;k;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;f;g;h;I;k;l;n;o;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;I;j;k;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;h;I;j;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;I;l;m;n;o;q</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1760,6 +2068,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1818,10 +2132,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2123,7 +2433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0E3DF6-783A-41F7-B1F8-4D6D60C1AEB8}">
   <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6115,10 +6427,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89DDA3-8E7F-45E5-9AF1-30B0C881C5E7}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="11145" topLeftCell="G1" activePane="topRight"/>
+      <selection activeCell="H4" sqref="H4"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6128,9 +6442,12 @@
     <col min="3" max="3" width="86.85546875" customWidth="1"/>
     <col min="4" max="4" width="40.140625" customWidth="1"/>
     <col min="5" max="5" width="103.28515625" customWidth="1"/>
+    <col min="6" max="6" width="96.85546875" customWidth="1"/>
+    <col min="7" max="7" width="100.5703125" customWidth="1"/>
+    <col min="8" max="8" width="111.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -6146,8 +6463,17 @@
       <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -6163,8 +6489,17 @@
       <c r="E2" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -6180,8 +6515,17 @@
       <c r="E3" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -6197,8 +6541,17 @@
       <c r="E4" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -6214,8 +6567,17 @@
       <c r="E5" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -6231,8 +6593,17 @@
       <c r="E6" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -6248,8 +6619,17 @@
       <c r="E7" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -6265,8 +6645,17 @@
       <c r="E8" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -6282,8 +6671,17 @@
       <c r="E9" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -6299,8 +6697,17 @@
       <c r="E10" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -6316,8 +6723,17 @@
       <c r="E11" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -6333,8 +6749,17 @@
       <c r="E12" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -6350,8 +6775,17 @@
       <c r="E13" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -6367,8 +6801,17 @@
       <c r="E14" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -6384,8 +6827,17 @@
       <c r="E15" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -6401,8 +6853,17 @@
       <c r="E16" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -6418,8 +6879,17 @@
       <c r="E17" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -6435,8 +6905,17 @@
       <c r="E18" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
     </row>
   </sheetData>
@@ -6447,13 +6926,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30BF69B-FB01-4D0C-BAF3-12969D5255D3}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2040" ySplit="600" topLeftCell="J1" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <pane xSplit="2040" topLeftCell="H1" activePane="topRight"/>
+      <selection pane="topRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6466,12 +6943,19 @@
     <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="85.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="26" width="27" customWidth="1"/>
+    <col min="27" max="27" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19" customWidth="1"/>
+    <col min="31" max="33" width="12" bestFit="1" customWidth="1"/>
+    <col min="34" max="38" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -6497,16 +6981,97 @@
         <v>111</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="AC1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -6531,17 +7096,17 @@
       <c r="H2" t="s">
         <v>122</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>123</v>
       </c>
-      <c r="J2" t="s">
+      <c r="AA2" t="s">
         <v>170</v>
       </c>
-      <c r="K2" t="s">
+      <c r="AB2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -6566,17 +7131,17 @@
       <c r="H3" t="s">
         <v>122</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>131</v>
       </c>
-      <c r="J3" t="s">
+      <c r="AA3" t="s">
         <v>176</v>
       </c>
-      <c r="K3" t="s">
+      <c r="AB3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -6601,17 +7166,32 @@
       <c r="H4" t="s">
         <v>122</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" t="s">
         <v>174</v>
       </c>
-      <c r="K4" t="s">
+      <c r="AB4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -6636,11 +7216,26 @@
       <c r="H5" t="s">
         <v>122</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -6665,11 +7260,11 @@
       <c r="H6" t="s">
         <v>122</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -6694,11 +7289,11 @@
       <c r="H7" t="s">
         <v>122</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -6723,11 +7318,11 @@
       <c r="H8" t="s">
         <v>122</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -6752,11 +7347,11 @@
       <c r="H9" t="s">
         <v>122</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -6781,11 +7376,11 @@
       <c r="H10" t="s">
         <v>148</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -6810,11 +7405,11 @@
       <c r="H11" t="s">
         <v>122</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -6839,11 +7434,11 @@
       <c r="H12" t="s">
         <v>122</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -6868,11 +7463,11 @@
       <c r="H13" t="s">
         <v>165</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -6897,11 +7492,26 @@
       <c r="H14" t="s">
         <v>122</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -6926,11 +7536,11 @@
       <c r="H15" t="s">
         <v>122</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -6955,11 +7565,11 @@
       <c r="H16" t="s">
         <v>197</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2022</v>
       </c>
@@ -6985,16 +7595,55 @@
         <v>122</v>
       </c>
       <c r="I17" t="s">
-        <v>123</v>
+        <v>241</v>
       </c>
       <c r="J17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K17" t="s">
+        <v>273</v>
+      </c>
+      <c r="L17" t="s">
+        <v>295</v>
+      </c>
+      <c r="M17" t="s">
+        <v>296</v>
+      </c>
+      <c r="N17" t="s">
+        <v>297</v>
+      </c>
+      <c r="O17" t="s">
+        <v>298</v>
+      </c>
+      <c r="P17" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>300</v>
+      </c>
+      <c r="R17" t="s">
+        <v>301</v>
+      </c>
+      <c r="AA17" t="s">
         <v>170</v>
       </c>
-      <c r="K17" t="s">
+      <c r="AB17" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="AC17" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>270</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2022</v>
       </c>
@@ -7014,13 +7663,28 @@
         <v>128</v>
       </c>
       <c r="G18" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="H18" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>241</v>
+      </c>
+      <c r="J18" t="s">
+        <v>303</v>
+      </c>
+      <c r="K18" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2022</v>
       </c>
@@ -7045,8 +7709,14 @@
       <c r="H19" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>304</v>
+      </c>
+      <c r="K19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2022</v>
       </c>
@@ -7072,16 +7742,22 @@
         <v>122</v>
       </c>
       <c r="I20" t="s">
+        <v>241</v>
+      </c>
+      <c r="J20" t="s">
+        <v>305</v>
+      </c>
+      <c r="K20" t="s">
         <v>203</v>
       </c>
-      <c r="J20" t="s">
+      <c r="AA20" t="s">
         <v>212</v>
       </c>
-      <c r="K20" t="s">
+      <c r="AB20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2022</v>
       </c>
@@ -7107,16 +7783,22 @@
         <v>122</v>
       </c>
       <c r="I21" t="s">
+        <v>241</v>
+      </c>
+      <c r="J21" t="s">
+        <v>306</v>
+      </c>
+      <c r="K21" t="s">
         <v>213</v>
       </c>
-      <c r="J21" t="s">
+      <c r="AA21" t="s">
         <v>214</v>
       </c>
-      <c r="K21" t="s">
+      <c r="AB21" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2022</v>
       </c>
@@ -7142,16 +7824,22 @@
         <v>122</v>
       </c>
       <c r="I22" t="s">
+        <v>241</v>
+      </c>
+      <c r="J22" t="s">
+        <v>307</v>
+      </c>
+      <c r="K22" t="s">
         <v>217</v>
       </c>
-      <c r="J22" t="s">
+      <c r="AA22" t="s">
         <v>218</v>
       </c>
-      <c r="K22" t="s">
+      <c r="AB22" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2022</v>
       </c>
@@ -7177,16 +7865,22 @@
         <v>122</v>
       </c>
       <c r="I23" t="s">
+        <v>241</v>
+      </c>
+      <c r="J23" t="s">
+        <v>308</v>
+      </c>
+      <c r="K23" t="s">
         <v>143</v>
       </c>
-      <c r="J23" t="s">
+      <c r="AA23" t="s">
         <v>216</v>
       </c>
-      <c r="K23" t="s">
+      <c r="AB23" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2022</v>
       </c>
@@ -7212,16 +7906,22 @@
         <v>122</v>
       </c>
       <c r="I24" t="s">
+        <v>241</v>
+      </c>
+      <c r="J24" t="s">
+        <v>309</v>
+      </c>
+      <c r="K24" t="s">
         <v>201</v>
       </c>
-      <c r="J24" t="s">
+      <c r="AA24" t="s">
         <v>220</v>
       </c>
-      <c r="K24" t="s">
+      <c r="AB24" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2022</v>
       </c>
@@ -7246,8 +7946,23 @@
       <c r="H25" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>241</v>
+      </c>
+      <c r="J25" t="s">
+        <v>305</v>
+      </c>
+      <c r="K25" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2022</v>
       </c>
@@ -7272,8 +7987,23 @@
       <c r="H26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>246</v>
+      </c>
+      <c r="J26" t="s">
+        <v>313</v>
+      </c>
+      <c r="K26" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2022</v>
       </c>
@@ -7298,8 +8028,23 @@
       <c r="H27" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>241</v>
+      </c>
+      <c r="J27" t="s">
+        <v>305</v>
+      </c>
+      <c r="K27" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2022</v>
       </c>
@@ -7324,8 +8069,23 @@
       <c r="H28" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>246</v>
+      </c>
+      <c r="J28" t="s">
+        <v>310</v>
+      </c>
+      <c r="K28" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2022</v>
       </c>
@@ -7350,8 +8110,23 @@
       <c r="H29" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>246</v>
+      </c>
+      <c r="J29" t="s">
+        <v>305</v>
+      </c>
+      <c r="K29" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>257</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2022</v>
       </c>
@@ -7376,8 +8151,23 @@
       <c r="H30" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>241</v>
+      </c>
+      <c r="J30" t="s">
+        <v>311</v>
+      </c>
+      <c r="K30" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2022</v>
       </c>
@@ -7402,8 +8192,24 @@
       <c r="H31" t="s">
         <v>197</v>
       </c>
+      <c r="I31" t="s">
+        <v>261</v>
+      </c>
+      <c r="J31" t="s">
+        <v>312</v>
+      </c>
+      <c r="K31" t="s">
+        <v>264</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>263</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{E225240A-263F-42B5-A61D-A1E352C93F0D}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{362BC566-C8A1-4659-BF44-C4905C2663EB}"/>

</xml_diff>

<commit_message>
* Paper outcomes functionality under paper summaries. * Mapping learning outcomes to BHealSc outcomes functionality. * Including this information in data file.
</commit_message>
<xml_diff>
--- a/2022 Major - Papers - Outcome Map.xlsx
+++ b/2022 Major - Papers - Outcome Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/BHealSc/Shared Documents/Scripts/Major Paper Outcomes Script/BHealSc Curriculum Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="730" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1178F0B5-DA58-4FF6-B86C-A829F7DDF848}"/>
+  <xr:revisionPtr revIDLastSave="790" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0D96CEA-8B5E-4722-9D5D-2471EF925B31}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="5" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
   </bookViews>
   <sheets>
     <sheet name="CMHC" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="328">
   <si>
     <t>Paper</t>
   </si>
@@ -2003,37 +2003,79 @@
     <t>BHealSc_Outcomes</t>
   </si>
   <si>
-    <t>a;b;c;d;e;f;g;h;I;j;l;m;n;o;p</t>
-  </si>
-  <si>
-    <t>a;b;c;d;f;g;h;I;m;n;o;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;f;g;h;I;j;k;l;m;n;o;p;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;f;g;h;I;j;l;m;n;o;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;g;h;I;j;l;m;n;o;p;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;g;h;I;k;l;m</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;g;h;I;k;l;m;n;o;p;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;f;g;h;I;k;l;n;o;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;g;h;I;j;k;l;m;n;o;p;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;h;I;j;l;m;n;o;p;q</t>
-  </si>
-  <si>
-    <t>a;b;c;d;e;g;h;I;l;m;n;o;q</t>
+    <t>a;b;c;d;e;f;g;h;i;j;k;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;f;g;h;i;j;l;m;n;o;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;i;j;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;i;k;l;m</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;i;k;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;i;l;m;n;o;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;f;g;h;i;k;l;n;o;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;g;h;i;j;k;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;h;i;j;l;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>Assignment 1 (2000 words); Presentation; Assignment 2 (2000 words); Final Exam (3-hr)</t>
+  </si>
+  <si>
+    <t>a;c;f;g;j;n</t>
+  </si>
+  <si>
+    <t>b;c;f;g;j;p</t>
+  </si>
+  <si>
+    <t>a;b;c;d;e;f;g;h;i;j;k;l;m;n;o;p</t>
+  </si>
+  <si>
+    <t>c;d;e;f;g;k</t>
+  </si>
+  <si>
+    <t>a;c;d;e;g;m;o</t>
+  </si>
+  <si>
+    <t>c;e;f;g;j</t>
+  </si>
+  <si>
+    <t>b;i;j;m</t>
+  </si>
+  <si>
+    <t>c;e;f;g;i;j;k</t>
+  </si>
+  <si>
+    <t>g;o</t>
+  </si>
+  <si>
+    <t>f;g</t>
+  </si>
+  <si>
+    <t>a;p</t>
+  </si>
+  <si>
+    <t>d;o;p</t>
+  </si>
+  <si>
+    <t>a;b;c;d;f;g;h;i;m;n;o;p;q</t>
+  </si>
+  <si>
+    <t>a;c;d</t>
+  </si>
+  <si>
+    <t>a;m</t>
   </si>
 </sst>
 </file>
@@ -2431,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0E3DF6-783A-41F7-B1F8-4D6D60C1AEB8}">
-  <dimension ref="A1:E138"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:B38"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,8 +2891,8 @@
       <c r="A49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>13</v>
+      <c r="B49" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2858,7 +2900,7 @@
         <v>24</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2866,7 +2908,7 @@
         <v>24</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2874,7 +2916,7 @@
         <v>24</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2882,15 +2924,15 @@
         <v>24</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2898,7 +2940,7 @@
         <v>25</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2906,7 +2948,7 @@
         <v>25</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2914,7 +2956,7 @@
         <v>25</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2922,7 +2964,7 @@
         <v>25</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2930,7 +2972,7 @@
         <v>25</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2938,7 +2980,7 @@
         <v>25</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2946,7 +2988,7 @@
         <v>25</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2954,7 +2996,7 @@
         <v>25</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2962,7 +3004,7 @@
         <v>25</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2970,7 +3012,7 @@
         <v>25</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2978,7 +3020,7 @@
         <v>25</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2986,7 +3028,7 @@
         <v>25</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2994,7 +3036,7 @@
         <v>25</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3002,15 +3044,15 @@
         <v>25</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3018,7 +3060,7 @@
         <v>27</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3026,7 +3068,7 @@
         <v>27</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3034,7 +3076,7 @@
         <v>27</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3042,7 +3084,7 @@
         <v>27</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3050,7 +3092,7 @@
         <v>27</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3058,7 +3100,7 @@
         <v>27</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3066,7 +3108,7 @@
         <v>27</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3074,7 +3116,7 @@
         <v>27</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3082,7 +3124,7 @@
         <v>27</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3090,15 +3132,15 @@
         <v>27</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3106,7 +3148,7 @@
         <v>28</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3114,7 +3156,7 @@
         <v>28</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3122,7 +3164,7 @@
         <v>28</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3130,7 +3172,7 @@
         <v>28</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3138,7 +3180,7 @@
         <v>28</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3146,7 +3188,7 @@
         <v>28</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3154,7 +3196,7 @@
         <v>28</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3162,7 +3204,7 @@
         <v>28</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3170,7 +3212,7 @@
         <v>28</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3178,7 +3220,7 @@
         <v>28</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3186,23 +3228,23 @@
         <v>28</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3210,7 +3252,7 @@
         <v>29</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3218,7 +3260,7 @@
         <v>29</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3226,7 +3268,7 @@
         <v>29</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3234,7 +3276,7 @@
         <v>29</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3242,7 +3284,7 @@
         <v>29</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3250,7 +3292,7 @@
         <v>29</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3258,7 +3300,7 @@
         <v>29</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3266,7 +3308,7 @@
         <v>29</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3274,7 +3316,7 @@
         <v>29</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3282,7 +3324,7 @@
         <v>29</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3290,7 +3332,7 @@
         <v>29</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3298,7 +3340,7 @@
         <v>29</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3306,7 +3348,7 @@
         <v>29</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3314,7 +3356,7 @@
         <v>29</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3322,23 +3364,23 @@
         <v>29</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3346,7 +3388,7 @@
         <v>30</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3354,7 +3396,7 @@
         <v>30</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3362,7 +3404,7 @@
         <v>30</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3370,7 +3412,7 @@
         <v>30</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3378,7 +3420,7 @@
         <v>30</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3386,7 +3428,7 @@
         <v>30</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3394,7 +3436,7 @@
         <v>30</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3402,7 +3444,7 @@
         <v>30</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3410,7 +3452,7 @@
         <v>30</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3418,7 +3460,7 @@
         <v>30</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3426,7 +3468,7 @@
         <v>30</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3434,7 +3476,7 @@
         <v>30</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3442,23 +3484,23 @@
         <v>30</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3466,7 +3508,7 @@
         <v>31</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3474,7 +3516,7 @@
         <v>31</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3482,7 +3524,7 @@
         <v>31</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3490,7 +3532,7 @@
         <v>31</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3498,7 +3540,7 @@
         <v>31</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3506,7 +3548,7 @@
         <v>31</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3514,7 +3556,7 @@
         <v>31</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3522,7 +3564,7 @@
         <v>31</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3530,7 +3572,7 @@
         <v>31</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3538,7 +3580,7 @@
         <v>31</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3546,7 +3588,7 @@
         <v>31</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3554,7 +3596,7 @@
         <v>31</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3562,6 +3604,22 @@
         <v>31</v>
       </c>
       <c r="B138" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3573,16 +3631,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12226758-8675-43FF-B095-EEA2A798FB0B}">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:B119"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="102.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.140625" customWidth="1"/>
     <col min="2" max="2" width="142.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3911,8 +3970,8 @@
       <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>12</v>
+      <c r="B39" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3920,15 +3979,15 @@
         <v>23</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3936,7 +3995,7 @@
         <v>25</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3944,7 +4003,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3952,7 +4011,7 @@
         <v>25</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3960,7 +4019,7 @@
         <v>25</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3968,7 +4027,7 @@
         <v>25</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3976,7 +4035,7 @@
         <v>25</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3984,7 +4043,7 @@
         <v>25</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3992,7 +4051,7 @@
         <v>25</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4000,7 +4059,7 @@
         <v>25</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4008,7 +4067,7 @@
         <v>25</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4016,7 +4075,7 @@
         <v>25</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4024,7 +4083,7 @@
         <v>25</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4032,7 +4091,7 @@
         <v>25</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4040,15 +4099,15 @@
         <v>25</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4056,7 +4115,7 @@
         <v>33</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4064,7 +4123,7 @@
         <v>33</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4072,7 +4131,7 @@
         <v>33</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4080,7 +4139,7 @@
         <v>33</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4088,7 +4147,7 @@
         <v>33</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4096,7 +4155,7 @@
         <v>33</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4104,7 +4163,7 @@
         <v>33</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4112,7 +4171,7 @@
         <v>33</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4120,7 +4179,7 @@
         <v>33</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4128,7 +4187,7 @@
         <v>33</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4136,7 +4195,7 @@
         <v>33</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4144,7 +4203,7 @@
         <v>33</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4152,7 +4211,7 @@
         <v>33</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4160,7 +4219,7 @@
         <v>33</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4168,15 +4227,15 @@
         <v>33</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4184,7 +4243,7 @@
         <v>34</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4192,7 +4251,7 @@
         <v>34</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4200,7 +4259,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4208,7 +4267,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4216,7 +4275,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4224,7 +4283,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4232,7 +4291,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4240,7 +4299,7 @@
         <v>34</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4248,7 +4307,7 @@
         <v>34</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4256,7 +4315,7 @@
         <v>34</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4264,7 +4323,7 @@
         <v>34</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4272,7 +4331,7 @@
         <v>34</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4280,7 +4339,7 @@
         <v>34</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4288,7 +4347,7 @@
         <v>34</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4296,15 +4355,15 @@
         <v>34</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4312,7 +4371,7 @@
         <v>30</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4320,7 +4379,7 @@
         <v>30</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4328,7 +4387,7 @@
         <v>30</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4336,7 +4395,7 @@
         <v>30</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4344,7 +4403,7 @@
         <v>30</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4352,7 +4411,7 @@
         <v>30</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4360,7 +4419,7 @@
         <v>30</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4368,7 +4427,7 @@
         <v>30</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4376,7 +4435,7 @@
         <v>30</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4384,7 +4443,7 @@
         <v>30</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4392,7 +4451,7 @@
         <v>30</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4400,7 +4459,7 @@
         <v>30</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4408,7 +4467,7 @@
         <v>30</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4416,15 +4475,15 @@
         <v>30</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4432,7 +4491,7 @@
         <v>35</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4440,7 +4499,7 @@
         <v>35</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4448,7 +4507,7 @@
         <v>35</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4456,7 +4515,7 @@
         <v>35</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4464,7 +4523,7 @@
         <v>35</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4472,7 +4531,7 @@
         <v>35</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4480,7 +4539,7 @@
         <v>35</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4488,7 +4547,7 @@
         <v>35</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4496,7 +4555,7 @@
         <v>35</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4504,7 +4563,7 @@
         <v>35</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4512,7 +4571,7 @@
         <v>35</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4520,7 +4579,7 @@
         <v>35</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4528,7 +4587,7 @@
         <v>35</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4536,7 +4595,7 @@
         <v>35</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4544,14 +4603,6 @@
         <v>35</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B119" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4565,7 +4616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE522F-2FAB-4701-B274-5C6971FD92B9}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A95" sqref="A95:B111"/>
     </sheetView>
   </sheetViews>
@@ -6430,7 +6481,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="11145" topLeftCell="G1" activePane="topRight"/>
+      <pane xSplit="11145" topLeftCell="C1" activePane="topRight"/>
       <selection activeCell="H4" sqref="H4"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -6929,8 +6980,9 @@
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2040" topLeftCell="H1" activePane="topRight"/>
-      <selection pane="topRight" activeCell="J27" sqref="J27"/>
+      <pane xSplit="2040" topLeftCell="N1" activePane="topRight"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection pane="topRight" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7672,10 +7724,37 @@
         <v>241</v>
       </c>
       <c r="J18" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="K18" t="s">
         <v>243</v>
+      </c>
+      <c r="L18" t="s">
+        <v>313</v>
+      </c>
+      <c r="M18" t="s">
+        <v>321</v>
+      </c>
+      <c r="N18" t="s">
+        <v>314</v>
+      </c>
+      <c r="O18" t="s">
+        <v>317</v>
+      </c>
+      <c r="P18" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>318</v>
+      </c>
+      <c r="R18" t="s">
+        <v>320</v>
+      </c>
+      <c r="S18" t="s">
+        <v>319</v>
+      </c>
+      <c r="T18" t="s">
+        <v>55</v>
       </c>
       <c r="AA18" t="s">
         <v>247</v>
@@ -7709,11 +7788,35 @@
       <c r="H19" t="s">
         <v>122</v>
       </c>
+      <c r="I19" t="s">
+        <v>241</v>
+      </c>
       <c r="J19" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="K19" t="s">
         <v>173</v>
+      </c>
+      <c r="L19" t="s">
+        <v>322</v>
+      </c>
+      <c r="M19" t="s">
+        <v>323</v>
+      </c>
+      <c r="N19" t="s">
+        <v>324</v>
+      </c>
+      <c r="O19" t="s">
+        <v>326</v>
+      </c>
+      <c r="P19" t="s">
+        <v>327</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>312</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -7745,7 +7848,7 @@
         <v>241</v>
       </c>
       <c r="J20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K20" t="s">
         <v>203</v>
@@ -7786,7 +7889,7 @@
         <v>241</v>
       </c>
       <c r="J21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K21" t="s">
         <v>213</v>
@@ -7827,7 +7930,7 @@
         <v>241</v>
       </c>
       <c r="J22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K22" t="s">
         <v>217</v>
@@ -7868,7 +7971,7 @@
         <v>241</v>
       </c>
       <c r="J23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K23" t="s">
         <v>143</v>
@@ -7909,7 +8012,7 @@
         <v>241</v>
       </c>
       <c r="J24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="K24" t="s">
         <v>201</v>
@@ -7950,7 +8053,7 @@
         <v>241</v>
       </c>
       <c r="J25" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K25" t="s">
         <v>244</v>
@@ -7991,7 +8094,7 @@
         <v>246</v>
       </c>
       <c r="J26" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="K26" t="s">
         <v>245</v>
@@ -8032,7 +8135,7 @@
         <v>241</v>
       </c>
       <c r="J27" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K27" t="s">
         <v>252</v>
@@ -8073,7 +8176,7 @@
         <v>246</v>
       </c>
       <c r="J28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K28" t="s">
         <v>253</v>
@@ -8114,7 +8217,7 @@
         <v>246</v>
       </c>
       <c r="J29" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K29" t="s">
         <v>256</v>
@@ -8155,7 +8258,7 @@
         <v>241</v>
       </c>
       <c r="J30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K30" t="s">
         <v>199</v>
@@ -8196,7 +8299,7 @@
         <v>261</v>
       </c>
       <c r="J31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K31" t="s">
         <v>264</v>
@@ -8248,26 +8351,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32cb602d-8189-4112-b11d-68ec1e0ac3d5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="dfbd8742-de2f-4d22-9c0e-7618d68088c2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE408B8C22746E499982C1BD963955F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab1bc5c41c46d57b3c0ab1580feb4c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32cb602d-8189-4112-b11d-68ec1e0ac3d5" xmlns:ns3="dfbd8742-de2f-4d22-9c0e-7618d68088c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="030a597698e86c278f656ea5c045ea7b" ns2:_="" ns3:_="">
     <xsd:import namespace="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
@@ -8504,32 +8587,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7E8779E-6CCC-4086-85C0-29701213007C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dfbd8742-de2f-4d22-9c0e-7618d68088c2"/>
-    <ds:schemaRef ds:uri="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32cb602d-8189-4112-b11d-68ec1e0ac3d5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dfbd8742-de2f-4d22-9c0e-7618d68088c2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ECABA6-DF96-42CB-A870-F92851FB0E4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8546,4 +8624,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7E8779E-6CCC-4086-85C0-29701213007C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dfbd8742-de2f-4d22-9c0e-7618d68088c2"/>
+    <ds:schemaRef ds:uri="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
* Removed learning outcome mappings for assessment. * Some small tidying up. * RC1 for GYR.
</commit_message>
<xml_diff>
--- a/2022 Major - Papers - Outcome Map.xlsx
+++ b/2022 Major - Papers - Outcome Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/BHealSc/Shared Documents/Scripts/Major Paper Outcomes Script/BHealSc Curriculum Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="994" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{443719A7-B819-4043-B428-7F42CC90700F}"/>
+  <xr:revisionPtr revIDLastSave="1012" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32820DBD-6B99-4235-B999-2E23926301EF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="393">
   <si>
     <t>Paper</t>
   </si>
@@ -2582,6 +2582,56 @@
 will be carried out and you will need to complete three interviews to pilot test your interview
 questions and briefly write up the results. While you may work in pairs, assignments are to be
 written up individually.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Whānau&lt;/b&gt;&lt;br /&gt;The concept of whānau and the role(s) that whānau and whānau members play to support the hauora of individuals and communities is central to Aotearoa New Zealand Māori health strategies and services. Working effectively with whānau is also a key expectation of health practitioners in Aotearoa.&lt;br&gt;&lt;br&gt;In this essay titled “Whānau” we would like you to:&lt;ol&gt;&lt;li&gt;Define and explain the concept of whānau&lt;/li&gt;&lt;li&gt;Describe and reflect on the role(s) that whānau play in contributing to the wellbeing of whānau members. Either use an example from literature and/or draw on your own experiences when answering this part of the essay&lt;/li&gt;&lt;li&gt;Reflect on and discuss how you would apply an aspect of what you have learnt about whānau, to working with Māori in health settings.&lt;/li&gt;&lt;/ol&gt;  </t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Cultural Competence or Racism Essay&lt;/b&gt;&lt;br /&gt;&lt;br&gt;&lt;b&gt;Cultural Competence&lt;/b&gt;&lt;br /&gt;Cultural competence and cultural safety have been highlighted as important for health practitioners, in order to achieve positive outcomes when working with Māori.&lt;ol&gt;&lt;li&gt;Using literature, please define and explain the concept of cultural safety as it applies to health care, within a New Zealand context.&lt;/li&gt;&lt;li&gt;Using literature, please define and explain the concept of cultural competence as it applies to health care, within a New Zealand context.&lt;/li&gt;&lt;li&gt;Describe and reflect on an approach you would use to create a culturally safe and responsive space for Māori, individuals and their whānau.&lt;/li&gt;&lt;/ol&gt;&lt;br&gt;&lt;br&gt;&lt;b&gt;Racism and Hauora Māori&lt;/b&gt;&lt;br /&gt;Racism has been linked to poor health outcomes for Māori. &lt;ol&gt;&lt;li&gt;Using literature, define and discuss the three levels of racism.&lt;/li&gt;&lt;li&gt;Using literature, discuss how ONE of the three levels of racism impacts on health outcomes for Māori individuals and their whānau&lt;/li&gt;&lt;li&gt;Reflect on and discuss ONE approach you would apply to address this level of racism when working with Māori in health settings.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Tamariki Ora and Health Literacy&lt;/b&gt;&lt;br /&gt;Your group has been asked by the local Māori health provider to assist them in their roles of supporting the health literacy of the community they work with.&lt;br&gt;
+Local kura, kōhanga and community members want to know more about how they can support the hauora of their pēpi, tamariki and rangatahi.&lt;br&gt;
+In order to do this, your group will research and develop a health literacy resource that focusses on your chosen health issue. You will then present this resource back to whānau and the community.&lt;br&gt;
+Getting a topic: Each group will pick from a choice of two topics (provided at the introduction to this assignment).&lt;br&gt;
+For your topic:&lt;ul&gt;&lt;li&gt;
+Do some research on this issue and its importance for Māori (how does it impact on Māori tamariki).&lt;/li&gt;&lt;li&gt;
+You should also identify some key messages about your health issue you think would be useful for whānau to know.&lt;/li&gt;&lt;/ul&gt;
+Based on what you learn about your topic:&lt;ol&gt;&lt;li&gt;
+Develop a resource that could be used by the community that provides relevant information on how they can best support the hauora of their pēpi, tamariki and/or rangatahi.&lt;/li&gt;&lt;li&gt;Prepare a 5-10 minute presentation on your topic to the audience who is made up of representatives from the local Māori health provider and key community stakeholders.
+&lt;i&gt;You will present your topic (explaining the health issue and the resource you have developed) during the tutorial time&lt;/i&gt;.&lt;/li&gt;&lt;li&gt;
+Upload a copy of your resource, your presentation and reflection .&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>In this essay we would like you to:&lt;ul&gt;&lt;li&gt;Describe what is meant by the term ‘Māori health provider’ and discuss common features of Māori health providers that arise in the literature.&lt;/li&gt;&lt;li&gt;
+Using an example, describe the specific strategies and approaches taken by one Māori health provider, to meet the needs of Māori.&lt;/li&gt;&lt;li&gt;Choose one health concern you believe will be an area of focus for Māori health providers in the future, and outline a potential role that Māori health providers could play in that area of focus.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Background:&lt;/b&gt; In MAOH301 the course objective is focused on how health services can make a difference for Māori health and eliminate inequity.  &lt;br&gt;
+A wide range of issues and approaches have been covered including: kaupapa Māori approaches, Māori health providers, incorporation of matauranga Māori and rongoā Māori, being responsive and addressing inequity, meeting Treaty expectations, health workforce etc etc.  We have also covered (or will soon cover) aspects such as vision, values, governance and strategic planning. &lt;br&gt;
+So, what would a service that met Māori needs and addressed inequity look like? Through this group assignment, you are going to show us!&lt;br&gt;
+&lt;b&gt;The scenario:&lt;/b&gt;  Health Aotearoa (NZ) had an evaluation completed which signalled a lack of responsiveness to Māori and there is provision for re-structuring. The Māori Health Funding Authority is tasked with leading the charge on identifying a number of priority areas to focus upon.  They have decided to seek expressions of interest from health providers for specific services.  The providers will be presenting their proposed services (via a presentation and briefing document) to the service provider selection panel. &lt;br&gt;
+&lt;b&gt;Your group task:&lt;/b&gt; Your group will pick out of 3 ‘future services’ and will choose one to be the focus of your assignment. &lt;br&gt;
+In your designated groups, we want you to design a service that will meet the needs of Māori focussed on the service you have chosen.&lt;br&gt;
+Your job is to prepare a proposal and present your proposal to a Health Aotearoa (NZ) / community representative panel (ie staff from Kōhatu) assessing the presentation.&lt;br&gt;
+Your proposal will be a presentation that is between 5 and 10 mins in whatever form you like.&lt;br&gt;
+Please include a briefing document outlining your proposal.&lt;br&gt;
+&lt;b&gt;Include in your presentation:&lt;/b&gt; &lt;ul&gt;&lt;li&gt;
+A description of your service&lt;/li&gt;&lt;li&gt;
+Why it is needed (you can research the area that your service is in, and describe its impact on Māori health, why services are needed etc)&lt;/li&gt;&lt;/ul&gt;
+&lt;b&gt;Please consider the following:&lt;/b&gt;&lt;ul&gt;&lt;li&gt;What will your service look like? e.g specific programmes/services&lt;/li&gt;&lt;li&gt;Outline your vision, values / principles and other areas e.g strategy, who are your stakeholders?&lt;/li&gt;&lt;li&gt;What will the Governance of your service look like and how will you be accountable for your outcomes?&lt;/li&gt;&lt;li&gt;How will you ensure responsiveness, address inequity and align with Te Tiriti o Waitangi?&lt;/li&gt;&lt;/ul&gt;
+&lt;b&gt;Template for your briefing document:&lt;/b&gt;&lt;br /&gt;
+The following provides a template for your briefing document (One-pager about your service) &lt;br&gt;
+Please include in your ‘one-page briefing’: &lt;br&gt;
+Name of your service &lt;br&gt;
+A description of your service&lt;br&gt;
+Rationale for your service - why it is needed?&lt;br&gt;
+What specific programmes will be included in your service?&lt;br&gt;
+Outline of your vision, values / principles and other areas e.g who for?  Strategy?&lt;br&gt;
+What will the Governance of your service look like and how will you be accountable for your outcomes?&lt;br&gt;
+How will you ensure responsiveness, address inequity, align with Tiriti o Waitangi?&lt;br&gt;
+Note: A briefing document is a one-page overview of your service that sets out what your service involves, the rationale of why it’s needed, what your vision, values and principles are, what your governance structure looks like and accountability for Māori health outcomes and aligning with te Tiriti o Waitangi.&lt;br&gt;
+</t>
   </si>
 </sst>
 </file>
@@ -7490,10 +7540,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30BF69B-FB01-4D0C-BAF3-12969D5255D3}">
   <dimension ref="A1:AR31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="2040" topLeftCell="AA1" activePane="topRight"/>
       <selection activeCell="A19" sqref="A19:XFD19"/>
-      <selection pane="topRight" activeCell="AG31" sqref="AD31:AG31"/>
+      <selection pane="topRight" activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8479,6 +8529,15 @@
       <c r="AC21" t="s">
         <v>303</v>
       </c>
+      <c r="AD21" t="s">
+        <v>388</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>389</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>390</v>
+      </c>
       <c r="AG21" t="s">
         <v>271</v>
       </c>
@@ -8526,6 +8585,12 @@
       <c r="AC22" t="s">
         <v>308</v>
       </c>
+      <c r="AD22" t="s">
+        <v>391</v>
+      </c>
+      <c r="AE22" s="5" t="s">
+        <v>392</v>
+      </c>
       <c r="AF22" t="s">
         <v>297</v>
       </c>
@@ -8916,7 +8981,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2022</v>
       </c>
@@ -8968,7 +9033,7 @@
       <c r="AF30" t="s">
         <v>382</v>
       </c>
-      <c r="AG30" s="2" t="s">
+      <c r="AG30" t="s">
         <v>383</v>
       </c>
       <c r="AH30" t="s">
@@ -9018,16 +9083,16 @@
       <c r="AC31" t="s">
         <v>349</v>
       </c>
-      <c r="AD31" s="5" t="s">
+      <c r="AD31" t="s">
         <v>384</v>
       </c>
-      <c r="AE31" s="5" t="s">
+      <c r="AE31" t="s">
         <v>385</v>
       </c>
-      <c r="AF31" s="5" t="s">
+      <c r="AF31" t="s">
         <v>386</v>
       </c>
-      <c r="AG31" s="5" t="s">
+      <c r="AG31" t="s">
         <v>387</v>
       </c>
     </row>
@@ -9082,15 +9147,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE408B8C22746E499982C1BD963955F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab1bc5c41c46d57b3c0ab1580feb4c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32cb602d-8189-4112-b11d-68ec1e0ac3d5" xmlns:ns3="dfbd8742-de2f-4d22-9c0e-7618d68088c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="030a597698e86c278f656ea5c045ea7b" ns2:_="" ns3:_="">
     <xsd:import namespace="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
@@ -9327,6 +9383,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7E8779E-6CCC-4086-85C0-29701213007C}">
   <ds:schemaRefs>
@@ -9339,14 +9404,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ECABA6-DF96-42CB-A870-F92851FB0E4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9363,4 +9420,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
* Reordered PAGH papers so that in alphabetical order on by major map.
</commit_message>
<xml_diff>
--- a/2022 Major - Papers - Outcome Map.xlsx
+++ b/2022 Major - Papers - Outcome Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/BHealSc/Shared Documents/Scripts/Major Paper Outcomes Script/BHealSc Curriculum Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1012" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32820DBD-6B99-4235-B999-2E23926301EF}"/>
+  <xr:revisionPtr revIDLastSave="1013" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CD77227-3A6F-4DF2-A742-2EB02FA39A53}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
   </bookViews>
   <sheets>
     <sheet name="CMHC" sheetId="1" r:id="rId1"/>
@@ -2704,7 +2704,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2714,7 +2714,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2731,10 +2730,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5177,8 +5172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE522F-2FAB-4701-B274-5C6971FD92B9}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:B111"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5381,7 +5376,7 @@
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>11</v>
@@ -5389,7 +5384,7 @@
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>
@@ -5397,7 +5392,7 @@
     </row>
     <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>13</v>
@@ -5405,7 +5400,7 @@
     </row>
     <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>14</v>
@@ -5413,7 +5408,7 @@
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>15</v>
@@ -5421,255 +5416,255 @@
     </row>
     <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>6</v>
@@ -5677,127 +5672,127 @@
     </row>
     <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>7</v>
@@ -5805,7 +5800,7 @@
     </row>
     <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>19</v>
@@ -5813,7 +5808,7 @@
     </row>
     <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>8</v>
@@ -7540,7 +7535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30BF69B-FB01-4D0C-BAF3-12969D5255D3}">
   <dimension ref="A1:AR31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <pane xSplit="2040" topLeftCell="AA1" activePane="topRight"/>
       <selection activeCell="A19" sqref="A19:XFD19"/>
       <selection pane="topRight" activeCell="AE22" sqref="AE22"/>
@@ -8588,7 +8583,7 @@
       <c r="AD22" t="s">
         <v>391</v>
       </c>
-      <c r="AE22" s="5" t="s">
+      <c r="AE22" t="s">
         <v>392</v>
       </c>
       <c r="AF22" t="s">
@@ -9147,6 +9142,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE408B8C22746E499982C1BD963955F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab1bc5c41c46d57b3c0ab1580feb4c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32cb602d-8189-4112-b11d-68ec1e0ac3d5" xmlns:ns3="dfbd8742-de2f-4d22-9c0e-7618d68088c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="030a597698e86c278f656ea5c045ea7b" ns2:_="" ns3:_="">
     <xsd:import namespace="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
@@ -9383,15 +9387,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7E8779E-6CCC-4086-85C0-29701213007C}">
   <ds:schemaRefs>
@@ -9404,6 +9399,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ECABA6-DF96-42CB-A870-F92851FB0E4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9420,12 +9423,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
* Fixed some typos.
</commit_message>
<xml_diff>
--- a/2022 Major - Papers - Outcome Map.xlsx
+++ b/2022 Major - Papers - Outcome Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/BHealSc/Shared Documents/Scripts/Major Paper Outcomes Script/BHealSc Curriculum Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1013" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CD77227-3A6F-4DF2-A742-2EB02FA39A53}"/>
+  <xr:revisionPtr revIDLastSave="1015" documentId="8_{E19A13B4-7705-4F0F-B970-DB8DAEF8FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C56943CE-E016-4A11-9EA7-0F39FB435B5A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{4FDA5C34-F275-4C05-A9ED-D24C57F0D6EC}"/>
   </bookViews>
   <sheets>
     <sheet name="CMHC" sheetId="1" r:id="rId1"/>
@@ -2080,17 +2080,11 @@
     <t>Demonstrate an understanding of the process and politics of health policymaking, including the main actors in the health policy process.;Demonstrate an understanding of frameworks for analysing health policy and health systems.;Demonstrate an understanding of different health systems and the various means by which health services are organised, funded and delivered in different countries.;Analyse and discuss various health policy issues and cases.</t>
   </si>
   <si>
-    <t>Assignment 1 (1500 words);A Assignment 2 (2000 words); Final Exam</t>
-  </si>
-  <si>
     <t>An introduction to Māori public health, exploring the nature and extent of the Māori population, determinants of Māori health outcomes, Māori health inequities and initiatives to address these.&lt;br&gt;
 This paper will provide you with an introduction to Māori health status and outcomes and the determinants of Māori health.  We will also develop an understanding of equity in health. A range of key public health issues will be discussed, outlining what the issue is, why it is important,  how this is being addressed, and what other opportunities to affect the issue could be adopted.</t>
   </si>
   <si>
     <t>Demonstrate an understanding of key historical processes, personalities and events relating to Hauora Māori and Hauora a Iwi/Māori public health.;Critically examine the impact of historical factors on contemporary Hauora Māori and Hauora a Iwi/Māori public health outcomes.Demonstrate an understanding of contemporary Hauora Māori and Hauora a Iwi/Māori public health.;Critically analyse and understand contemporary Hauora Māori topics and public health approaches to addressing inequities.</t>
-  </si>
-  <si>
-    <t>Online Quiz; Group Presenation; Online Quiz; Assignment; Final Exam</t>
   </si>
   <si>
     <t>10%;15%;10%;25%;40%</t>
@@ -2632,6 +2626,12 @@
 How will you ensure responsiveness, address inequity, align with Tiriti o Waitangi?&lt;br&gt;
 Note: A briefing document is a one-page overview of your service that sets out what your service involves, the rationale of why it’s needed, what your vision, values and principles are, what your governance structure looks like and accountability for Māori health outcomes and aligning with te Tiriti o Waitangi.&lt;br&gt;
 </t>
+  </si>
+  <si>
+    <t>Assignment 1 (1500 words);Assignment 2 (2000 words); Final Exam</t>
+  </si>
+  <si>
+    <t>Online Quiz; Group Presentation; Online Quiz; Assignment; Final Exam</t>
   </si>
 </sst>
 </file>
@@ -2730,6 +2730,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5172,7 +5176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE522F-2FAB-4701-B274-5C6971FD92B9}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
@@ -7037,7 +7041,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane xSplit="11145" topLeftCell="C1" activePane="topRight"/>
+      <pane xSplit="11145" topLeftCell="H1" activePane="topRight"/>
       <selection activeCell="H4" sqref="H4"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -7535,10 +7539,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30BF69B-FB01-4D0C-BAF3-12969D5255D3}">
   <dimension ref="A1:AR31"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2040" topLeftCell="AA1" activePane="topRight"/>
       <selection activeCell="A19" sqref="A19:XFD19"/>
-      <selection pane="topRight" activeCell="AE22" sqref="AE22"/>
+      <selection pane="topRight" activeCell="AB28" sqref="AB28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8348,10 +8352,10 @@
         <v>190</v>
       </c>
       <c r="AD18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AE18" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AF18" t="s">
         <v>271</v>
@@ -8416,13 +8420,13 @@
         <v>195</v>
       </c>
       <c r="AD19" t="s">
+        <v>350</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>351</v>
+      </c>
+      <c r="AF19" t="s">
         <v>352</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>353</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>354</v>
       </c>
       <c r="AG19" t="s">
         <v>271</v>
@@ -8472,10 +8476,10 @@
         <v>190</v>
       </c>
       <c r="AD20" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AE20" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AF20" t="s">
         <v>297</v>
@@ -8525,13 +8529,13 @@
         <v>303</v>
       </c>
       <c r="AD21" t="s">
+        <v>386</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>387</v>
+      </c>
+      <c r="AF21" t="s">
         <v>388</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>389</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>390</v>
       </c>
       <c r="AG21" t="s">
         <v>271</v>
@@ -8581,10 +8585,10 @@
         <v>308</v>
       </c>
       <c r="AD22" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AE22" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AF22" t="s">
         <v>297</v>
@@ -8634,13 +8638,13 @@
         <v>303</v>
       </c>
       <c r="AD23" t="s">
+        <v>355</v>
+      </c>
+      <c r="AE23" t="s">
         <v>357</v>
       </c>
-      <c r="AE23" t="s">
-        <v>359</v>
-      </c>
       <c r="AF23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AG23" t="s">
         <v>271</v>
@@ -8684,19 +8688,19 @@
         <v>216</v>
       </c>
       <c r="AB24" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AC24" t="s">
         <v>303</v>
       </c>
       <c r="AD24" t="s">
+        <v>358</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>359</v>
+      </c>
+      <c r="AF24" t="s">
         <v>360</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>361</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>362</v>
       </c>
       <c r="AG24" t="s">
         <v>297</v>
@@ -8740,16 +8744,16 @@
         <v>318</v>
       </c>
       <c r="AB25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AC25" t="s">
         <v>308</v>
       </c>
       <c r="AD25" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AE25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AF25" t="s">
         <v>271</v>
@@ -8793,16 +8797,16 @@
         <v>322</v>
       </c>
       <c r="AB26" t="s">
-        <v>323</v>
+        <v>391</v>
       </c>
       <c r="AC26" t="s">
         <v>308</v>
       </c>
       <c r="AD26" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AE26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AF26" t="s">
         <v>271</v>
@@ -8834,7 +8838,7 @@
         <v>178</v>
       </c>
       <c r="I27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J27" t="s">
         <v>258</v>
@@ -8843,28 +8847,28 @@
         <v>295</v>
       </c>
       <c r="L27" t="s">
+        <v>324</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>392</v>
+      </c>
+      <c r="AC27" t="s">
         <v>325</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AD27" t="s">
+        <v>364</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>365</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>370</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>366</v>
+      </c>
+      <c r="AH27" t="s">
         <v>326</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>327</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>366</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>367</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>372</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>368</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
@@ -8881,7 +8885,7 @@
         <v>174</v>
       </c>
       <c r="E28" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>236</v>
@@ -8893,31 +8897,31 @@
         <v>238</v>
       </c>
       <c r="I28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J28" t="s">
         <v>320</v>
       </c>
       <c r="K28" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AB28" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AC28" t="s">
+        <v>373</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>371</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>372</v>
+      </c>
+      <c r="AF28" t="s">
         <v>375</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>373</v>
-      </c>
-      <c r="AE28" t="s">
-        <v>374</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>377</v>
       </c>
       <c r="AG28" t="s">
         <v>271</v>
@@ -8937,10 +8941,10 @@
         <v>184</v>
       </c>
       <c r="E29" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G29" t="s">
         <v>233</v>
@@ -8949,7 +8953,7 @@
         <v>178</v>
       </c>
       <c r="I29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J29" t="s">
         <v>320</v>
@@ -8958,19 +8962,19 @@
         <v>295</v>
       </c>
       <c r="L29" t="s">
+        <v>334</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>335</v>
+      </c>
+      <c r="AC29" t="s">
         <v>336</v>
       </c>
-      <c r="AB29" t="s">
-        <v>337</v>
-      </c>
-      <c r="AC29" t="s">
-        <v>338</v>
-      </c>
       <c r="AD29" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AE29" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AF29" t="s">
         <v>271</v>
@@ -9002,34 +9006,34 @@
         <v>178</v>
       </c>
       <c r="I30" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="J30" t="s">
         <v>258</v>
       </c>
       <c r="K30" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L30" t="s">
         <v>250</v>
       </c>
       <c r="AB30" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AC30" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AD30" t="s">
+        <v>378</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>379</v>
+      </c>
+      <c r="AF30" t="s">
         <v>380</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AG30" t="s">
         <v>381</v>
-      </c>
-      <c r="AF30" t="s">
-        <v>382</v>
-      </c>
-      <c r="AG30" t="s">
-        <v>383</v>
       </c>
       <c r="AH30" t="s">
         <v>297</v>
@@ -9049,7 +9053,7 @@
         <v>174</v>
       </c>
       <c r="E31" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>254</v>
@@ -9061,34 +9065,34 @@
         <v>255</v>
       </c>
       <c r="I31" t="s">
+        <v>342</v>
+      </c>
+      <c r="J31" t="s">
+        <v>343</v>
+      </c>
+      <c r="K31" t="s">
         <v>344</v>
       </c>
-      <c r="J31" t="s">
+      <c r="L31" t="s">
         <v>345</v>
       </c>
-      <c r="K31" t="s">
+      <c r="AB31" t="s">
         <v>346</v>
       </c>
-      <c r="L31" t="s">
+      <c r="AC31" t="s">
         <v>347</v>
       </c>
-      <c r="AB31" t="s">
-        <v>348</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>349</v>
-      </c>
       <c r="AD31" t="s">
+        <v>382</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>383</v>
+      </c>
+      <c r="AF31" t="s">
         <v>384</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AG31" t="s">
         <v>385</v>
-      </c>
-      <c r="AF31" t="s">
-        <v>386</v>
-      </c>
-      <c r="AG31" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -9131,26 +9135,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32cb602d-8189-4112-b11d-68ec1e0ac3d5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="dfbd8742-de2f-4d22-9c0e-7618d68088c2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE408B8C22746E499982C1BD963955F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab1bc5c41c46d57b3c0ab1580feb4c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="32cb602d-8189-4112-b11d-68ec1e0ac3d5" xmlns:ns3="dfbd8742-de2f-4d22-9c0e-7618d68088c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="030a597698e86c278f656ea5c045ea7b" ns2:_="" ns3:_="">
     <xsd:import namespace="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
@@ -9387,26 +9371,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7E8779E-6CCC-4086-85C0-29701213007C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
-    <ds:schemaRef ds:uri="dfbd8742-de2f-4d22-9c0e-7618d68088c2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="32cb602d-8189-4112-b11d-68ec1e0ac3d5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dfbd8742-de2f-4d22-9c0e-7618d68088c2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ECABA6-DF96-42CB-A870-F92851FB0E4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9423,4 +9408,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FD82B2-CC7E-457F-9565-D834CF718525}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7E8779E-6CCC-4086-85C0-29701213007C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="32cb602d-8189-4112-b11d-68ec1e0ac3d5"/>
+    <ds:schemaRef ds:uri="dfbd8742-de2f-4d22-9c0e-7618d68088c2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>